<commit_message>
update bom linear rail
</commit_message>
<xml_diff>
--- a/BOM/Gripper_BOM.xlsx
+++ b/BOM/Gripper_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="List 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Screws and nuts:</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Linear guide</t>
+  </si>
+  <si>
+    <t>100mm</t>
   </si>
   <si>
     <t>Magnet</t>
@@ -571,412 +574,411 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="7" max="7" width="31.75"/>
-    <col customWidth="1" min="8" max="8" width="24.13"/>
-    <col customWidth="1" min="9" max="9" width="23.88"/>
-    <col customWidth="1" min="10" max="10" width="27.25"/>
+    <col customWidth="1" min="6" max="6" width="51.88"/>
   </cols>
   <sheetData>
-    <row r="7">
-      <c r="G7" s="1" t="s">
+    <row r="12">
+      <c r="F12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="G8" s="3" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="F13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="G9" s="5" t="s">
+      <c r="I13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="6">
+      <c r="G14" s="6">
         <v>4.0</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10">
-      <c r="G10" s="8" t="s">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15">
+      <c r="F15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="9">
+      <c r="G15" s="9">
         <v>8.0</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11">
-      <c r="G11" s="5" t="s">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16">
+      <c r="F16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="6">
+      <c r="G16" s="6">
         <v>5.0</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12">
-      <c r="G12" s="8" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="F17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="G13" s="5" t="s">
+      <c r="G17" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18">
+      <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="6">
+      <c r="G18" s="6">
         <v>7.0</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14">
-      <c r="G14" s="8" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19">
+      <c r="F19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="9">
+      <c r="G19" s="9">
         <v>4.0</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15">
-      <c r="G15" s="5" t="s">
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20">
+      <c r="F20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="6">
+      <c r="G20" s="6">
         <v>4.0</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="G16" s="8" t="s">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21">
+      <c r="F21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="9">
+      <c r="G21" s="9">
         <v>4.0</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="G17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22">
+      <c r="F22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="6">
         <v>3.0</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18">
-      <c r="G18" s="11" t="s">
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23">
+      <c r="F23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19">
-      <c r="G19" s="5" t="s">
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24">
+      <c r="F24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="G20" s="8" t="s">
+      <c r="G24" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="F25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="9">
+      <c r="G25" s="9">
         <v>15.0</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="G21" s="15" t="s">
+      <c r="H25" s="10"/>
+      <c r="I25" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="F26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="G22" s="3" t="s">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27">
+      <c r="F27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="G27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="G23" s="5" t="s">
+      <c r="I27" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="F28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="G24" s="18" t="s">
+      <c r="G28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="F29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-    </row>
-    <row r="25">
-      <c r="G25" s="20" t="s">
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30">
+      <c r="F30" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="G30" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="H30" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="G26" s="8" t="s">
+      <c r="I30" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="F31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="G31" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="G27" s="5" t="s">
+      <c r="I31" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="F32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="6">
+      <c r="G32" s="6">
         <v>2.0</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="G28" s="8" t="s">
+      <c r="H32" s="7"/>
+      <c r="I32" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="F33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="G29" s="5" t="s">
+      <c r="G33" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H33" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I29" s="7" t="s">
+      <c r="I33" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30">
-      <c r="G30" s="23" t="s">
+      <c r="G34" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-    </row>
-    <row r="31">
-      <c r="G31" s="20" t="s">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35">
+      <c r="F35" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36">
+      <c r="F36" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="G36" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="H36" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="G32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="I36" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="F37" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="G33" s="5" t="s">
+      <c r="G37" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I33" s="7" t="s">
+      <c r="I37" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="F38" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="G34" s="8" t="s">
+      <c r="G38" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I34" s="10" t="s">
+      <c r="I38" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="G35" s="5" t="s">
+      <c r="G39" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H39" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I35" s="13" t="s">
+      <c r="I39" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="G36" s="25" t="s">
+      <c r="G40" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H40" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-    </row>
-    <row r="37">
-      <c r="G37" s="5" t="s">
+      <c r="I40" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="F41" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42">
+      <c r="F42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="G38" s="8" t="s">
+      <c r="H42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H38" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="G39" s="5" t="s">
+      <c r="I42" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="F43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J39" s="13" t="s">
+      <c r="G43" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="F44" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="13" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J19"/>
-    <hyperlink r:id="rId2" ref="J20"/>
-    <hyperlink r:id="rId3" ref="I23"/>
-    <hyperlink r:id="rId4" ref="J23"/>
-    <hyperlink r:id="rId5" ref="J26"/>
-    <hyperlink r:id="rId6" ref="J27"/>
-    <hyperlink r:id="rId7" ref="J28"/>
-    <hyperlink r:id="rId8" ref="I32"/>
-    <hyperlink r:id="rId9" ref="J32"/>
-    <hyperlink r:id="rId10" ref="J33"/>
-    <hyperlink r:id="rId11" ref="J34"/>
-    <hyperlink r:id="rId12" ref="I35"/>
-    <hyperlink r:id="rId13" ref="J35"/>
-    <hyperlink r:id="rId14" ref="J37"/>
-    <hyperlink r:id="rId15" ref="I38"/>
-    <hyperlink r:id="rId16" ref="J38"/>
-    <hyperlink r:id="rId17" ref="I39"/>
-    <hyperlink r:id="rId18" ref="J39"/>
+    <hyperlink r:id="rId1" ref="I24"/>
+    <hyperlink r:id="rId2" ref="I25"/>
+    <hyperlink r:id="rId3" ref="H28"/>
+    <hyperlink r:id="rId4" ref="I28"/>
+    <hyperlink r:id="rId5" ref="I31"/>
+    <hyperlink r:id="rId6" ref="I32"/>
+    <hyperlink r:id="rId7" ref="I33"/>
+    <hyperlink r:id="rId8" ref="H37"/>
+    <hyperlink r:id="rId9" ref="I37"/>
+    <hyperlink r:id="rId10" ref="I38"/>
+    <hyperlink r:id="rId11" ref="I39"/>
+    <hyperlink r:id="rId12" ref="H40"/>
+    <hyperlink r:id="rId13" ref="I40"/>
+    <hyperlink r:id="rId14" ref="I42"/>
+    <hyperlink r:id="rId15" ref="H43"/>
+    <hyperlink r:id="rId16" ref="I43"/>
+    <hyperlink r:id="rId17" ref="H44"/>
+    <hyperlink r:id="rId18" ref="I44"/>
   </hyperlinks>
   <drawing r:id="rId19"/>
 </worksheet>

</xml_diff>